<commit_message>
[KWR002] update template + fix max row template (50) : #102446
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR002.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR002.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UK\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5322F45B-D44F-4633-A75C-4F454CA00843}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BA346B-B3D5-4E90-9899-233B5A4BE5E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21660" windowHeight="4755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">template!$A$1:$BJ$17</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -73,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +117,18 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="ＭＳ ゴシック"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="ＭＳ ゴシック"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -626,7 +641,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
@@ -644,7 +659,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -655,45 +669,15 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -712,6 +696,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -724,38 +756,119 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
@@ -763,94 +876,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -875,15 +907,6 @@
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -903,6 +926,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1222,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="B1" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="AW17" sqref="AW17"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="9.75" customHeight="1"/>
@@ -1232,15 +1258,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
       <c r="H1" s="45" t="s">
         <v>2</v>
       </c>
@@ -1256,148 +1282,148 @@
       <c r="R1" s="47"/>
       <c r="S1" s="47"/>
       <c r="T1" s="47"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="14"/>
+      <c r="AQ1" s="23"/>
+      <c r="AR1" s="21"/>
       <c r="AS1" s="12"/>
       <c r="AT1" s="13"/>
       <c r="AU1" s="12"/>
       <c r="AV1" s="13"/>
-      <c r="AW1" s="9"/>
-      <c r="AX1" s="11"/>
-      <c r="AY1" s="9"/>
-      <c r="AZ1" s="11"/>
-      <c r="BA1" s="9"/>
-      <c r="BB1" s="11"/>
-      <c r="BC1" s="9"/>
-      <c r="BD1" s="11"/>
-      <c r="BE1" s="9"/>
-      <c r="BF1" s="11"/>
-      <c r="BG1" s="9"/>
-      <c r="BH1" s="11"/>
-      <c r="BI1" s="9"/>
-      <c r="BJ1" s="10"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="10"/>
+      <c r="BC1" s="8"/>
+      <c r="BD1" s="10"/>
+      <c r="BE1" s="8"/>
+      <c r="BF1" s="10"/>
+      <c r="BG1" s="8"/>
+      <c r="BH1" s="10"/>
+      <c r="BI1" s="8"/>
+      <c r="BJ1" s="9"/>
     </row>
     <row r="2" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="45" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="45" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="AQ2" s="17"/>
-      <c r="AR2" s="15"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="AQ2" s="24"/>
+      <c r="AR2" s="22"/>
       <c r="AS2" s="12"/>
       <c r="AT2" s="13"/>
       <c r="AU2" s="12"/>
       <c r="AV2" s="13"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="11"/>
-      <c r="AY2" s="9"/>
-      <c r="AZ2" s="11"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="11"/>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="11"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="11"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="11"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="10"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="8"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="8"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="8"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="8"/>
+      <c r="BJ2" s="9"/>
     </row>
     <row r="3" spans="1:62" ht="9.75" customHeight="1">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
     </row>
     <row r="4" spans="1:62" ht="9.75" customHeight="1">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="58" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="93"/>
-      <c r="T4" s="94"/>
-      <c r="U4" s="40"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="42"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="42"/>
-      <c r="Z4" s="44"/>
-      <c r="AD4" s="24"/>
-      <c r="AE4" s="24"/>
-      <c r="AF4" s="24"/>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="24"/>
-      <c r="AI4" s="24"/>
-      <c r="AJ4" s="24"/>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="24"/>
-      <c r="AM4" s="24"/>
-      <c r="AN4" s="24"/>
-      <c r="AO4" s="24"/>
-      <c r="AQ4" s="70"/>
-      <c r="AR4" s="72"/>
-      <c r="AS4" s="74"/>
-      <c r="AT4" s="74"/>
-      <c r="AU4" s="74"/>
-      <c r="AV4" s="74"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="95"/>
+      <c r="T4" s="96"/>
+      <c r="U4" s="54"/>
+      <c r="V4" s="55"/>
+      <c r="W4" s="56"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="56"/>
+      <c r="Z4" s="58"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20"/>
+      <c r="AH4" s="20"/>
+      <c r="AI4" s="20"/>
+      <c r="AJ4" s="20"/>
+      <c r="AK4" s="20"/>
+      <c r="AL4" s="20"/>
+      <c r="AM4" s="20"/>
+      <c r="AN4" s="20"/>
+      <c r="AO4" s="20"/>
+      <c r="AQ4" s="74"/>
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="25"/>
+      <c r="AT4" s="25"/>
+      <c r="AU4" s="25"/>
+      <c r="AV4" s="25"/>
       <c r="AW4" s="48"/>
       <c r="AX4" s="49"/>
       <c r="AY4" s="48"/>
@@ -1411,55 +1437,55 @@
       <c r="BG4" s="48"/>
       <c r="BH4" s="49"/>
       <c r="BI4" s="48"/>
-      <c r="BJ4" s="54"/>
+      <c r="BJ4" s="61"/>
     </row>
     <row r="5" spans="1:62" ht="9.75" customHeight="1">
-      <c r="A5" s="89"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="40" t="s">
+      <c r="A5" s="91"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="40"/>
-      <c r="X5" s="41"/>
-      <c r="Y5" s="40"/>
-      <c r="Z5" s="53"/>
-      <c r="AD5" s="24"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="24"/>
-      <c r="AI5" s="24"/>
-      <c r="AJ5" s="24"/>
-      <c r="AK5" s="24"/>
-      <c r="AL5" s="24"/>
-      <c r="AM5" s="24"/>
-      <c r="AN5" s="24"/>
-      <c r="AO5" s="24"/>
-      <c r="AQ5" s="71"/>
-      <c r="AR5" s="73"/>
-      <c r="AS5" s="74"/>
-      <c r="AT5" s="74"/>
-      <c r="AU5" s="74"/>
-      <c r="AV5" s="74"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="55"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="54"/>
+      <c r="V5" s="55"/>
+      <c r="W5" s="54"/>
+      <c r="X5" s="55"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="60"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="20"/>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="20"/>
+      <c r="AN5" s="20"/>
+      <c r="AO5" s="20"/>
+      <c r="AQ5" s="75"/>
+      <c r="AR5" s="77"/>
+      <c r="AS5" s="25"/>
+      <c r="AT5" s="25"/>
+      <c r="AU5" s="25"/>
+      <c r="AV5" s="25"/>
       <c r="AW5" s="48"/>
       <c r="AX5" s="49"/>
       <c r="AY5" s="48"/>
@@ -1473,51 +1499,51 @@
       <c r="BG5" s="48"/>
       <c r="BH5" s="49"/>
       <c r="BI5" s="48"/>
-      <c r="BJ5" s="54"/>
+      <c r="BJ5" s="61"/>
     </row>
     <row r="6" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A6" s="89"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="55"/>
-      <c r="V6" s="56"/>
-      <c r="W6" s="55"/>
-      <c r="X6" s="56"/>
-      <c r="Y6" s="55"/>
-      <c r="Z6" s="57"/>
-      <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="24"/>
-      <c r="AI6" s="24"/>
-      <c r="AJ6" s="24"/>
-      <c r="AK6" s="24"/>
-      <c r="AL6" s="24"/>
-      <c r="AM6" s="24"/>
-      <c r="AN6" s="24"/>
-      <c r="AO6" s="24"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="51"/>
+      <c r="S6" s="50"/>
+      <c r="T6" s="51"/>
+      <c r="U6" s="50"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="50"/>
+      <c r="X6" s="51"/>
+      <c r="Y6" s="50"/>
+      <c r="Z6" s="62"/>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
+      <c r="AI6" s="20"/>
+      <c r="AJ6" s="20"/>
+      <c r="AK6" s="20"/>
+      <c r="AL6" s="20"/>
+      <c r="AM6" s="20"/>
+      <c r="AN6" s="20"/>
+      <c r="AO6" s="20"/>
     </row>
     <row r="7" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A7" s="91"/>
-      <c r="B7" s="92"/>
+      <c r="A7" s="93"/>
+      <c r="B7" s="94"/>
       <c r="C7" s="48"/>
       <c r="D7" s="49"/>
       <c r="E7" s="48"/>
@@ -1541,261 +1567,282 @@
       <c r="W7" s="48"/>
       <c r="X7" s="49"/>
       <c r="Y7" s="48"/>
-      <c r="Z7" s="54"/>
-      <c r="AD7" s="24"/>
-      <c r="AE7" s="24"/>
-      <c r="AF7" s="24"/>
-      <c r="AG7" s="24"/>
-      <c r="AH7" s="24"/>
-      <c r="AI7" s="24"/>
-      <c r="AJ7" s="24"/>
-      <c r="AK7" s="24"/>
-      <c r="AL7" s="24"/>
-      <c r="AM7" s="24"/>
-      <c r="AN7" s="24"/>
-      <c r="AO7" s="24"/>
-      <c r="AQ7" s="45" t="s">
+      <c r="Z7" s="61"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="20"/>
+      <c r="AL7" s="20"/>
+      <c r="AM7" s="20"/>
+      <c r="AN7" s="20"/>
+      <c r="AO7" s="20"/>
+      <c r="AQ7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AR7" s="46"/>
-      <c r="AS7" s="47"/>
-      <c r="AT7" s="47"/>
-      <c r="AU7" s="47"/>
-      <c r="AV7" s="47"/>
-      <c r="AW7" s="47"/>
-      <c r="AX7" s="45" t="s">
+      <c r="AR7" s="78"/>
+      <c r="AS7" s="79"/>
+      <c r="AT7" s="79"/>
+      <c r="AU7" s="79"/>
+      <c r="AV7" s="79"/>
+      <c r="AW7" s="79"/>
+      <c r="AX7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="AY7" s="46"/>
-      <c r="AZ7" s="47"/>
-      <c r="BA7" s="47"/>
-      <c r="BB7" s="47"/>
-      <c r="BC7" s="47"/>
-      <c r="BD7" s="47"/>
-      <c r="BE7" s="47"/>
-      <c r="BF7" s="47"/>
-      <c r="BG7" s="47"/>
-      <c r="BH7" s="47"/>
-      <c r="BI7" s="47"/>
-      <c r="BJ7" s="47"/>
+      <c r="AY7" s="78"/>
+      <c r="AZ7" s="79"/>
+      <c r="BA7" s="79"/>
+      <c r="BB7" s="79"/>
+      <c r="BC7" s="79"/>
+      <c r="BD7" s="79"/>
+      <c r="BE7" s="79"/>
+      <c r="BF7" s="79"/>
+      <c r="BG7" s="79"/>
+      <c r="BH7" s="79"/>
+      <c r="BI7" s="79"/>
+      <c r="BJ7" s="79"/>
     </row>
     <row r="8" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
       <c r="U8" s="1"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="27"/>
-      <c r="Y8" s="27"/>
-      <c r="Z8" s="27"/>
-      <c r="AA8" s="25"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="27"/>
-      <c r="AD8" s="27"/>
-      <c r="AE8" s="27"/>
-      <c r="AF8" s="25"/>
-      <c r="AG8" s="26"/>
-      <c r="AH8" s="26"/>
-      <c r="AI8" s="27"/>
-      <c r="AJ8" s="27"/>
-      <c r="AK8" s="27"/>
-      <c r="AL8" s="28"/>
-      <c r="AM8" s="29"/>
-      <c r="AN8" s="30"/>
-      <c r="AO8" s="30"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="16"/>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
+      <c r="AI8" s="16"/>
+      <c r="AJ8" s="16"/>
+      <c r="AK8" s="16"/>
+      <c r="AL8" s="17"/>
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="19"/>
+      <c r="AO8" s="19"/>
     </row>
     <row r="9" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="36"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="50"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="30"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="22" t="s">
+      <c r="V9" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="W9" s="35" t="s">
+      <c r="W9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X9" s="21" t="s">
+      <c r="X9" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="22"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="21"/>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="22"/>
-      <c r="AH9" s="21"/>
-      <c r="AI9" s="22"/>
-      <c r="AJ9" s="21"/>
-      <c r="AK9" s="22"/>
-      <c r="AL9" s="21"/>
-      <c r="AM9" s="22"/>
-      <c r="AN9" s="21"/>
-      <c r="AO9" s="23"/>
-      <c r="AQ9" s="45" t="s">
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="26"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="27"/>
+      <c r="AD9" s="26"/>
+      <c r="AE9" s="27"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="26"/>
+      <c r="AI9" s="27"/>
+      <c r="AJ9" s="26"/>
+      <c r="AK9" s="27"/>
+      <c r="AL9" s="26"/>
+      <c r="AM9" s="27"/>
+      <c r="AN9" s="26"/>
+      <c r="AO9" s="35"/>
+      <c r="AQ9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="AR9" s="46"/>
-      <c r="AS9" s="47"/>
-      <c r="AT9" s="47"/>
-      <c r="AU9" s="47"/>
-      <c r="AV9" s="45" t="s">
+      <c r="AR9" s="78"/>
+      <c r="AS9" s="79"/>
+      <c r="AT9" s="79"/>
+      <c r="AU9" s="79"/>
+      <c r="AV9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="AW9" s="46"/>
-      <c r="AX9" s="47"/>
-      <c r="AY9" s="47"/>
-      <c r="AZ9" s="47"/>
-      <c r="BA9" s="45" t="s">
+      <c r="AW9" s="78"/>
+      <c r="AX9" s="79"/>
+      <c r="AY9" s="79"/>
+      <c r="AZ9" s="79"/>
+      <c r="BA9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="BB9" s="46"/>
-      <c r="BC9" s="46"/>
-      <c r="BD9" s="47"/>
-      <c r="BE9" s="47"/>
-      <c r="BF9" s="47"/>
-      <c r="BG9" s="45" t="s">
+      <c r="BB9" s="78"/>
+      <c r="BC9" s="78"/>
+      <c r="BD9" s="79"/>
+      <c r="BE9" s="79"/>
+      <c r="BF9" s="79"/>
+      <c r="BG9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="BH9" s="46"/>
-      <c r="BI9" s="47"/>
-      <c r="BJ9" s="47"/>
+      <c r="BH9" s="78"/>
+      <c r="BI9" s="79"/>
+      <c r="BJ9" s="79"/>
     </row>
     <row r="10" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A10" s="32"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="37" t="s">
+      <c r="A10" s="37"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="52"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="59"/>
       <c r="U10" s="3"/>
-      <c r="V10" s="51"/>
-      <c r="W10" s="39"/>
-      <c r="X10" s="18" t="s">
+      <c r="V10" s="31"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="18"/>
-      <c r="AG10" s="19"/>
-      <c r="AH10" s="18"/>
-      <c r="AI10" s="19"/>
-      <c r="AJ10" s="18"/>
-      <c r="AK10" s="19"/>
-      <c r="AL10" s="18"/>
-      <c r="AM10" s="19"/>
-      <c r="AN10" s="18"/>
-      <c r="AO10" s="20"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="32"/>
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="32"/>
+      <c r="AC10" s="33"/>
+      <c r="AD10" s="32"/>
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="32"/>
+      <c r="AG10" s="33"/>
+      <c r="AH10" s="32"/>
+      <c r="AI10" s="33"/>
+      <c r="AJ10" s="32"/>
+      <c r="AK10" s="33"/>
+      <c r="AL10" s="32"/>
+      <c r="AM10" s="33"/>
+      <c r="AN10" s="32"/>
+      <c r="AO10" s="34"/>
     </row>
     <row r="11" spans="1:62" ht="9.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="AQ11" s="60" t="s">
+      <c r="AQ11" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="AR11" s="61"/>
+      <c r="AR11" s="65"/>
       <c r="AS11" s="4"/>
       <c r="AT11" s="4"/>
       <c r="AU11" s="4"/>
       <c r="AV11" s="4"/>
       <c r="AW11" s="4"/>
       <c r="AX11" s="4"/>
-      <c r="AY11" s="81"/>
-      <c r="AZ11" s="81"/>
-      <c r="BA11" s="81"/>
-      <c r="BB11" s="81"/>
-      <c r="BC11" s="81"/>
-      <c r="BD11" s="82"/>
-      <c r="BE11" s="83"/>
-      <c r="BF11" s="84"/>
-      <c r="BG11" s="83"/>
-      <c r="BH11" s="84"/>
-      <c r="BI11" s="83"/>
-      <c r="BJ11" s="85"/>
+      <c r="AY11" s="86"/>
+      <c r="AZ11" s="86"/>
+      <c r="BA11" s="86"/>
+      <c r="BB11" s="86"/>
+      <c r="BC11" s="86"/>
+      <c r="BD11" s="87"/>
+      <c r="BE11" s="88"/>
+      <c r="BF11" s="89"/>
+      <c r="BG11" s="88"/>
+      <c r="BH11" s="89"/>
+      <c r="BI11" s="88"/>
+      <c r="BJ11" s="90"/>
     </row>
     <row r="12" spans="1:62" ht="9.75" customHeight="1" thickTop="1">
-      <c r="AQ12" s="75"/>
-      <c r="AR12" s="75"/>
+      <c r="AQ12" s="80"/>
+      <c r="AR12" s="80"/>
       <c r="AS12" s="5"/>
       <c r="AT12" s="5"/>
       <c r="AU12" s="5"/>
       <c r="AV12" s="5"/>
       <c r="AW12" s="5"/>
       <c r="AX12" s="5"/>
-      <c r="AY12" s="76"/>
-      <c r="AZ12" s="76"/>
-      <c r="BA12" s="76"/>
-      <c r="BB12" s="76"/>
-      <c r="BC12" s="76"/>
-      <c r="BD12" s="77"/>
-      <c r="BE12" s="78"/>
-      <c r="BF12" s="79"/>
-      <c r="BG12" s="78"/>
-      <c r="BH12" s="79"/>
-      <c r="BI12" s="78"/>
-      <c r="BJ12" s="80"/>
+      <c r="AY12" s="81"/>
+      <c r="AZ12" s="81"/>
+      <c r="BA12" s="81"/>
+      <c r="BB12" s="81"/>
+      <c r="BC12" s="81"/>
+      <c r="BD12" s="82"/>
+      <c r="BE12" s="83"/>
+      <c r="BF12" s="84"/>
+      <c r="BG12" s="83"/>
+      <c r="BH12" s="84"/>
+      <c r="BI12" s="83"/>
+      <c r="BJ12" s="85"/>
     </row>
     <row r="14" spans="1:62" ht="9.75" customHeight="1">
-      <c r="AQ14" s="62"/>
-      <c r="AR14" s="63"/>
+      <c r="AQ14" s="66"/>
+      <c r="AR14" s="67"/>
     </row>
     <row r="15" spans="1:62" ht="9.75" customHeight="1">
-      <c r="AQ15" s="64"/>
-      <c r="AR15" s="65"/>
+      <c r="AQ15" s="68"/>
+      <c r="AR15" s="69"/>
     </row>
     <row r="16" spans="1:62" ht="9.75" customHeight="1">
-      <c r="AQ16" s="66"/>
-      <c r="AR16" s="67"/>
+      <c r="AQ16" s="70"/>
+      <c r="AR16" s="71"/>
     </row>
     <row r="17" spans="43:44" ht="9.75" customHeight="1">
-      <c r="AQ17" s="68"/>
-      <c r="AR17" s="69"/>
+      <c r="AQ17" s="72"/>
+      <c r="AR17" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="173">
+    <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="BE4:BF4"/>
+    <mergeCell ref="BG4:BH4"/>
+    <mergeCell ref="BI4:BJ4"/>
+    <mergeCell ref="BG11:BH11"/>
+    <mergeCell ref="BI11:BJ11"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="A4:B7"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
@@ -1803,30 +1850,10 @@
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="BA4:BB4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="BE4:BF4"/>
-    <mergeCell ref="BG4:BH4"/>
-    <mergeCell ref="BI4:BJ4"/>
-    <mergeCell ref="BG11:BH11"/>
-    <mergeCell ref="BI11:BJ11"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AW5:AX5"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="A4:B7"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="BG12:BH12"/>
     <mergeCell ref="BI12:BJ12"/>
     <mergeCell ref="BC5:BD5"/>
     <mergeCell ref="BE5:BF5"/>
@@ -1836,9 +1863,10 @@
     <mergeCell ref="BA11:BB11"/>
     <mergeCell ref="BC11:BD11"/>
     <mergeCell ref="BE11:BF11"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:Y9"/>
     <mergeCell ref="AQ11:AR11"/>
     <mergeCell ref="AY4:AZ4"/>
     <mergeCell ref="AQ14:AR14"/>
@@ -1859,17 +1887,6 @@
     <mergeCell ref="BA12:BB12"/>
     <mergeCell ref="BC12:BD12"/>
     <mergeCell ref="BE12:BF12"/>
-    <mergeCell ref="BG12:BH12"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="X10:Y10"/>
-    <mergeCell ref="Z10:AA10"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA8:AE8"/>
     <mergeCell ref="AB9:AC9"/>
     <mergeCell ref="AD9:AE9"/>
     <mergeCell ref="Y7:Z7"/>
@@ -1881,12 +1898,7 @@
     <mergeCell ref="S5:T5"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="S7:T7"/>
-    <mergeCell ref="AD4:AE4"/>
     <mergeCell ref="AD5:AE7"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:T1"/>
     <mergeCell ref="V8:Z8"/>
@@ -1905,10 +1917,12 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="AF9:AG9"/>
-    <mergeCell ref="AF10:AG10"/>
-    <mergeCell ref="AB10:AC10"/>
-    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="U5:V5"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:D9"/>
@@ -1925,15 +1939,30 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="Z9:AA9"/>
     <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AH4:AI4"/>
-    <mergeCell ref="AJ4:AK4"/>
-    <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="AH10:AI10"/>
+    <mergeCell ref="AJ10:AK10"/>
+    <mergeCell ref="AL10:AM10"/>
+    <mergeCell ref="AN10:AO10"/>
+    <mergeCell ref="AH9:AI9"/>
+    <mergeCell ref="AJ9:AK9"/>
+    <mergeCell ref="AL9:AM9"/>
+    <mergeCell ref="AN9:AO9"/>
+    <mergeCell ref="AF9:AG9"/>
+    <mergeCell ref="AF10:AG10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="Z10:AA10"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA8:AE8"/>
     <mergeCell ref="AF8:AK8"/>
     <mergeCell ref="AL8:AO8"/>
     <mergeCell ref="AF5:AG7"/>
@@ -1943,16 +1972,9 @@
     <mergeCell ref="AN5:AO7"/>
     <mergeCell ref="AR1:AR2"/>
     <mergeCell ref="AQ1:AQ2"/>
-    <mergeCell ref="AH10:AI10"/>
-    <mergeCell ref="AJ10:AK10"/>
-    <mergeCell ref="AL10:AM10"/>
-    <mergeCell ref="AN10:AO10"/>
-    <mergeCell ref="AH9:AI9"/>
-    <mergeCell ref="AJ9:AK9"/>
-    <mergeCell ref="AL9:AM9"/>
-    <mergeCell ref="AN9:AO9"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AJ4:AK4"/>
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="AN4:AO4"/>
     <mergeCell ref="BE1:BF1"/>
     <mergeCell ref="BC1:BD1"/>
     <mergeCell ref="BA1:BB1"/>
@@ -1969,6 +1991,10 @@
     <mergeCell ref="BA2:BB2"/>
     <mergeCell ref="AY2:AZ2"/>
     <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AS2:AT2"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <printOptions horizontalCentered="1"/>
@@ -1979,7 +2005,7 @@
 page&amp;P</oddHeader>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="48" max="16383" man="1"/>
+    <brk id="50" max="61" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="41" max="1048575" man="1"/>

</xml_diff>

<commit_message>
update KWR002 giai thuat in an
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR002.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR002.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\KWR002 Sua excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21660" windowHeight="4755"/>
   </bookViews>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">template!$A$1:$BJ$17</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,8 +74,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +133,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -149,7 +161,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -361,17 +373,6 @@
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="medium">
         <color auto="1"/>
@@ -559,6 +560,62 @@
         <color indexed="64"/>
       </top>
       <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -572,7 +629,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
@@ -585,17 +642,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -607,10 +664,10 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -625,30 +682,33 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="33" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="32" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="33" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="34" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -657,10 +717,7 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="35" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="36" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -669,6 +726,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -684,20 +744,17 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
@@ -717,7 +774,7 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="33" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="32" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -729,13 +786,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -759,7 +816,10 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="36" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -768,32 +828,32 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="38" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="39" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1104,7 +1164,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1114,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:J4"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7:AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="9.75" customHeight="1"/>
@@ -1434,6 +1494,8 @@
       <c r="X7" s="17"/>
       <c r="Y7" s="15"/>
       <c r="Z7" s="16"/>
+      <c r="AB7" s="76"/>
+      <c r="AC7" s="76"/>
       <c r="AD7" s="12"/>
       <c r="AE7" s="12"/>
       <c r="AF7" s="12"/>
@@ -1494,7 +1556,7 @@
       <c r="AN8" s="75"/>
       <c r="AO8" s="75"/>
     </row>
-    <row r="9" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
+    <row r="9" spans="1:62" ht="12.2" customHeight="1" thickBot="1">
       <c r="A9" s="59" t="s">
         <v>7</v>
       </c>
@@ -1520,34 +1582,34 @@
       <c r="Q9" s="63"/>
       <c r="R9" s="63"/>
       <c r="S9" s="63"/>
-      <c r="T9" s="65"/>
+      <c r="T9" s="66"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="66" t="s">
+      <c r="V9" s="67" t="s">
         <v>7</v>
       </c>
       <c r="W9" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="X9" s="65" t="s">
+      <c r="X9" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="66"/>
-      <c r="Z9" s="65"/>
-      <c r="AA9" s="66"/>
-      <c r="AB9" s="65"/>
-      <c r="AC9" s="66"/>
-      <c r="AD9" s="65"/>
-      <c r="AE9" s="66"/>
-      <c r="AF9" s="65"/>
-      <c r="AG9" s="66"/>
-      <c r="AH9" s="65"/>
-      <c r="AI9" s="66"/>
-      <c r="AJ9" s="65"/>
-      <c r="AK9" s="66"/>
-      <c r="AL9" s="65"/>
-      <c r="AM9" s="66"/>
-      <c r="AN9" s="65"/>
-      <c r="AO9" s="71"/>
+      <c r="Y9" s="67"/>
+      <c r="Z9" s="66"/>
+      <c r="AA9" s="67"/>
+      <c r="AB9" s="66"/>
+      <c r="AC9" s="67"/>
+      <c r="AD9" s="66"/>
+      <c r="AE9" s="67"/>
+      <c r="AF9" s="66"/>
+      <c r="AG9" s="67"/>
+      <c r="AH9" s="66"/>
+      <c r="AI9" s="67"/>
+      <c r="AJ9" s="66"/>
+      <c r="AK9" s="67"/>
+      <c r="AL9" s="66"/>
+      <c r="AM9" s="67"/>
+      <c r="AN9" s="66"/>
+      <c r="AO9" s="69"/>
       <c r="AQ9" s="44" t="s">
         <v>3</v>
       </c>
@@ -1577,10 +1639,10 @@
       <c r="BI9" s="46"/>
       <c r="BJ9" s="46"/>
     </row>
-    <row r="10" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
+    <row r="10" spans="1:62" ht="12.2" customHeight="1" thickBot="1">
       <c r="A10" s="60"/>
       <c r="B10" s="62"/>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="65" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="64"/>
@@ -1599,30 +1661,30 @@
       <c r="Q10" s="64"/>
       <c r="R10" s="64"/>
       <c r="S10" s="64"/>
-      <c r="T10" s="68"/>
+      <c r="T10" s="70"/>
       <c r="U10" s="3"/>
-      <c r="V10" s="67"/>
+      <c r="V10" s="68"/>
       <c r="W10" s="72"/>
-      <c r="X10" s="68" t="s">
+      <c r="X10" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="Y10" s="69"/>
-      <c r="Z10" s="68"/>
-      <c r="AA10" s="69"/>
-      <c r="AB10" s="68"/>
-      <c r="AC10" s="69"/>
-      <c r="AD10" s="68"/>
-      <c r="AE10" s="69"/>
-      <c r="AF10" s="68"/>
-      <c r="AG10" s="69"/>
-      <c r="AH10" s="68"/>
-      <c r="AI10" s="69"/>
-      <c r="AJ10" s="68"/>
-      <c r="AK10" s="69"/>
-      <c r="AL10" s="68"/>
-      <c r="AM10" s="69"/>
-      <c r="AN10" s="68"/>
-      <c r="AO10" s="70"/>
+      <c r="Y10" s="71"/>
+      <c r="Z10" s="64"/>
+      <c r="AA10" s="64"/>
+      <c r="AB10" s="64"/>
+      <c r="AC10" s="64"/>
+      <c r="AD10" s="64"/>
+      <c r="AE10" s="64"/>
+      <c r="AF10" s="64"/>
+      <c r="AG10" s="64"/>
+      <c r="AH10" s="64"/>
+      <c r="AI10" s="64"/>
+      <c r="AJ10" s="64"/>
+      <c r="AK10" s="64"/>
+      <c r="AL10" s="64"/>
+      <c r="AM10" s="64"/>
+      <c r="AN10" s="64"/>
+      <c r="AO10" s="64"/>
     </row>
     <row r="11" spans="1:62" ht="9.75" customHeight="1" thickTop="1">
       <c r="AQ11" s="31" t="s">
@@ -1674,20 +1736,20 @@
       <c r="AQ14" s="32"/>
       <c r="AR14" s="33"/>
     </row>
-    <row r="15" spans="1:62" ht="9.75" customHeight="1">
+    <row r="15" spans="1:62" ht="11.45" customHeight="1">
       <c r="AQ15" s="34"/>
       <c r="AR15" s="35"/>
     </row>
-    <row r="16" spans="1:62" ht="9.75" customHeight="1">
+    <row r="16" spans="1:62" ht="11.45" customHeight="1">
       <c r="AQ16" s="36"/>
       <c r="AR16" s="37"/>
     </row>
-    <row r="17" spans="43:44" ht="9.75" customHeight="1">
+    <row r="17" spans="43:44" ht="11.45" customHeight="1">
       <c r="AQ17" s="38"/>
       <c r="AR17" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="173">
+  <mergeCells count="174">
     <mergeCell ref="BI2:BJ2"/>
     <mergeCell ref="BG2:BH2"/>
     <mergeCell ref="BE2:BF2"/>
@@ -1722,6 +1784,7 @@
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="AN4:AO4"/>
     <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="AB7:AC7"/>
     <mergeCell ref="Z9:AA9"/>
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="S9:T9"/>
@@ -1867,8 +1930,8 @@
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.31496062992126"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;9&amp;=$companyName&amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16&amp;=$reportName&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;9&amp;D　&amp;T　
-page&amp;P</oddHeader>
+    <oddHeader>&amp;L&amp;=$companyName&amp;C&amp;"ＭＳ ゴシック,標準"&amp;16&amp;=$reportName&amp;R&amp;"ＭＳ ゴシック,標準"&amp;9&amp;D　&amp;T　
+&amp;=I18N.KWR002_210(bean)&amp;P</oddHeader>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="50" max="61" man="1"/>

</xml_diff>

<commit_message>
fix template + column
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR002.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR002.xlsx
@@ -758,7 +758,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
@@ -788,17 +788,38 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -806,15 +827,27 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
@@ -833,9 +866,6 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -848,10 +878,28 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -905,35 +953,8 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -947,7 +968,13 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="17" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -986,38 +1013,8 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1340,7 +1337,7 @@
   <dimension ref="A1:BJ17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="175" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="M10" sqref="M10:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="9.75" customHeight="1"/>
@@ -1394,26 +1391,26 @@
       <c r="AM1" s="7"/>
       <c r="AN1" s="7"/>
       <c r="AO1" s="7"/>
-      <c r="AQ1" s="73"/>
-      <c r="AR1" s="71"/>
-      <c r="AS1" s="76"/>
-      <c r="AT1" s="77"/>
-      <c r="AU1" s="76"/>
-      <c r="AV1" s="77"/>
-      <c r="AW1" s="76"/>
-      <c r="AX1" s="77"/>
-      <c r="AY1" s="76"/>
-      <c r="AZ1" s="77"/>
-      <c r="BA1" s="76"/>
-      <c r="BB1" s="77"/>
-      <c r="BC1" s="76"/>
-      <c r="BD1" s="77"/>
-      <c r="BE1" s="76"/>
-      <c r="BF1" s="77"/>
-      <c r="BG1" s="76"/>
-      <c r="BH1" s="77"/>
-      <c r="BI1" s="76"/>
-      <c r="BJ1" s="78"/>
+      <c r="AQ1" s="82"/>
+      <c r="AR1" s="80"/>
+      <c r="AS1" s="85"/>
+      <c r="AT1" s="86"/>
+      <c r="AU1" s="85"/>
+      <c r="AV1" s="86"/>
+      <c r="AW1" s="85"/>
+      <c r="AX1" s="86"/>
+      <c r="AY1" s="85"/>
+      <c r="AZ1" s="86"/>
+      <c r="BA1" s="85"/>
+      <c r="BB1" s="86"/>
+      <c r="BC1" s="85"/>
+      <c r="BD1" s="86"/>
+      <c r="BE1" s="85"/>
+      <c r="BF1" s="86"/>
+      <c r="BG1" s="85"/>
+      <c r="BH1" s="86"/>
+      <c r="BI1" s="85"/>
+      <c r="BJ1" s="87"/>
     </row>
     <row r="2" spans="1:62" ht="9.75" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -1439,51 +1436,51 @@
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AQ2" s="74"/>
-      <c r="AR2" s="72"/>
-      <c r="AS2" s="76"/>
-      <c r="AT2" s="77"/>
-      <c r="AU2" s="76"/>
-      <c r="AV2" s="77"/>
-      <c r="AW2" s="76"/>
-      <c r="AX2" s="77"/>
-      <c r="AY2" s="76"/>
-      <c r="AZ2" s="77"/>
-      <c r="BA2" s="76"/>
-      <c r="BB2" s="77"/>
-      <c r="BC2" s="76"/>
-      <c r="BD2" s="77"/>
-      <c r="BE2" s="76"/>
-      <c r="BF2" s="77"/>
-      <c r="BG2" s="76"/>
-      <c r="BH2" s="77"/>
-      <c r="BI2" s="76"/>
-      <c r="BJ2" s="78"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AQ2" s="83"/>
+      <c r="AR2" s="81"/>
+      <c r="AS2" s="85"/>
+      <c r="AT2" s="86"/>
+      <c r="AU2" s="85"/>
+      <c r="AV2" s="86"/>
+      <c r="AW2" s="85"/>
+      <c r="AX2" s="86"/>
+      <c r="AY2" s="85"/>
+      <c r="AZ2" s="86"/>
+      <c r="BA2" s="85"/>
+      <c r="BB2" s="86"/>
+      <c r="BC2" s="85"/>
+      <c r="BD2" s="86"/>
+      <c r="BE2" s="85"/>
+      <c r="BF2" s="86"/>
+      <c r="BG2" s="85"/>
+      <c r="BH2" s="86"/>
+      <c r="BI2" s="85"/>
+      <c r="BJ2" s="87"/>
     </row>
     <row r="3" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79" t="s">
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -1496,454 +1493,456 @@
       <c r="T3" s="8"/>
     </row>
     <row r="4" spans="1:62" ht="9.75" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="20" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="55"/>
-      <c r="AD4" s="16"/>
-      <c r="AE4" s="16"/>
-      <c r="AF4" s="16"/>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="16"/>
-      <c r="AO4" s="16"/>
-      <c r="AQ4" s="41"/>
-      <c r="AR4" s="43"/>
-      <c r="AS4" s="14"/>
-      <c r="AT4" s="15"/>
-      <c r="AU4" s="14"/>
-      <c r="AV4" s="15"/>
-      <c r="AW4" s="14"/>
-      <c r="AX4" s="15"/>
-      <c r="AY4" s="14"/>
-      <c r="AZ4" s="15"/>
-      <c r="BA4" s="14"/>
-      <c r="BB4" s="15"/>
-      <c r="BC4" s="14"/>
-      <c r="BD4" s="15"/>
-      <c r="BE4" s="14"/>
-      <c r="BF4" s="15"/>
-      <c r="BG4" s="14"/>
-      <c r="BH4" s="15"/>
-      <c r="BI4" s="14"/>
-      <c r="BJ4" s="22"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="49"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="17"/>
+      <c r="AJ4" s="17"/>
+      <c r="AK4" s="17"/>
+      <c r="AL4" s="17"/>
+      <c r="AM4" s="17"/>
+      <c r="AN4" s="17"/>
+      <c r="AO4" s="17"/>
+      <c r="AQ4" s="57"/>
+      <c r="AR4" s="59"/>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="14"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="14"/>
+      <c r="AW4" s="13"/>
+      <c r="AX4" s="14"/>
+      <c r="AY4" s="13"/>
+      <c r="AZ4" s="14"/>
+      <c r="BA4" s="13"/>
+      <c r="BB4" s="14"/>
+      <c r="BC4" s="13"/>
+      <c r="BD4" s="14"/>
+      <c r="BE4" s="13"/>
+      <c r="BF4" s="14"/>
+      <c r="BG4" s="13"/>
+      <c r="BH4" s="14"/>
+      <c r="BI4" s="13"/>
+      <c r="BJ4" s="33"/>
     </row>
     <row r="5" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="83" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
-      <c r="S5" s="83"/>
-      <c r="T5" s="84"/>
-      <c r="U5" s="83"/>
-      <c r="V5" s="84"/>
-      <c r="W5" s="83"/>
-      <c r="X5" s="84"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="85"/>
-      <c r="AD5" s="16"/>
-      <c r="AE5" s="16"/>
-      <c r="AF5" s="16"/>
-      <c r="AG5" s="16"/>
-      <c r="AH5" s="16"/>
-      <c r="AI5" s="16"/>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="16"/>
-      <c r="AL5" s="16"/>
-      <c r="AM5" s="16"/>
-      <c r="AN5" s="16"/>
-      <c r="AO5" s="16"/>
-      <c r="AQ5" s="42"/>
-      <c r="AR5" s="44"/>
-      <c r="AS5" s="14"/>
-      <c r="AT5" s="15"/>
-      <c r="AU5" s="14"/>
-      <c r="AV5" s="15"/>
-      <c r="AW5" s="14"/>
-      <c r="AX5" s="15"/>
-      <c r="AY5" s="14"/>
-      <c r="AZ5" s="15"/>
-      <c r="BA5" s="14"/>
-      <c r="BB5" s="15"/>
-      <c r="BC5" s="14"/>
-      <c r="BD5" s="15"/>
-      <c r="BE5" s="14"/>
-      <c r="BF5" s="15"/>
-      <c r="BG5" s="14"/>
-      <c r="BH5" s="15"/>
-      <c r="BI5" s="14"/>
-      <c r="BJ5" s="22"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="29"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="17"/>
+      <c r="AK5" s="17"/>
+      <c r="AL5" s="17"/>
+      <c r="AM5" s="17"/>
+      <c r="AN5" s="17"/>
+      <c r="AO5" s="17"/>
+      <c r="AQ5" s="58"/>
+      <c r="AR5" s="60"/>
+      <c r="AS5" s="13"/>
+      <c r="AT5" s="14"/>
+      <c r="AU5" s="13"/>
+      <c r="AV5" s="14"/>
+      <c r="AW5" s="13"/>
+      <c r="AX5" s="14"/>
+      <c r="AY5" s="13"/>
+      <c r="AZ5" s="14"/>
+      <c r="BA5" s="13"/>
+      <c r="BB5" s="14"/>
+      <c r="BC5" s="13"/>
+      <c r="BD5" s="14"/>
+      <c r="BE5" s="13"/>
+      <c r="BF5" s="14"/>
+      <c r="BG5" s="13"/>
+      <c r="BH5" s="14"/>
+      <c r="BI5" s="13"/>
+      <c r="BJ5" s="33"/>
     </row>
     <row r="6" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A6" s="58"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="80"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="80"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="80"/>
-      <c r="V6" s="81"/>
-      <c r="W6" s="80"/>
-      <c r="X6" s="81"/>
-      <c r="Y6" s="80"/>
-      <c r="Z6" s="82"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="16"/>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="16"/>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="16"/>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="16"/>
-      <c r="AL6" s="16"/>
-      <c r="AM6" s="16"/>
-      <c r="AN6" s="16"/>
-      <c r="AO6" s="16"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="28"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="17"/>
+      <c r="AG6" s="17"/>
+      <c r="AH6" s="17"/>
+      <c r="AI6" s="17"/>
+      <c r="AJ6" s="17"/>
+      <c r="AK6" s="17"/>
+      <c r="AL6" s="17"/>
+      <c r="AM6" s="17"/>
+      <c r="AN6" s="17"/>
+      <c r="AO6" s="17"/>
     </row>
     <row r="7" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
-      <c r="A7" s="60"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="19"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="18"/>
-      <c r="AB7" s="75"/>
-      <c r="AC7" s="75"/>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="16"/>
-      <c r="AF7" s="16"/>
-      <c r="AG7" s="16"/>
-      <c r="AH7" s="16"/>
-      <c r="AI7" s="16"/>
-      <c r="AJ7" s="16"/>
-      <c r="AK7" s="16"/>
-      <c r="AL7" s="16"/>
-      <c r="AM7" s="16"/>
-      <c r="AN7" s="16"/>
-      <c r="AO7" s="16"/>
-      <c r="AQ7" s="45" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="24"/>
+      <c r="Z7" s="25"/>
+      <c r="AB7" s="84"/>
+      <c r="AC7" s="84"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="17"/>
+      <c r="AF7" s="17"/>
+      <c r="AG7" s="17"/>
+      <c r="AH7" s="17"/>
+      <c r="AI7" s="17"/>
+      <c r="AJ7" s="17"/>
+      <c r="AK7" s="17"/>
+      <c r="AL7" s="17"/>
+      <c r="AM7" s="17"/>
+      <c r="AN7" s="17"/>
+      <c r="AO7" s="17"/>
+      <c r="AQ7" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="AR7" s="45"/>
-      <c r="AS7" s="45"/>
-      <c r="AT7" s="45"/>
-      <c r="AU7" s="45"/>
-      <c r="AV7" s="45"/>
-      <c r="AW7" s="45"/>
-      <c r="AX7" s="45" t="s">
+      <c r="AR7" s="61"/>
+      <c r="AS7" s="61"/>
+      <c r="AT7" s="61"/>
+      <c r="AU7" s="61"/>
+      <c r="AV7" s="61"/>
+      <c r="AW7" s="61"/>
+      <c r="AX7" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="AY7" s="45"/>
-      <c r="AZ7" s="45"/>
-      <c r="BA7" s="45"/>
-      <c r="BB7" s="45"/>
-      <c r="BC7" s="45"/>
-      <c r="BD7" s="45"/>
-      <c r="BE7" s="45"/>
-      <c r="BF7" s="45"/>
-      <c r="BG7" s="45"/>
-      <c r="BH7" s="45"/>
-      <c r="BI7" s="45"/>
-      <c r="BJ7" s="45"/>
+      <c r="AY7" s="61"/>
+      <c r="AZ7" s="61"/>
+      <c r="BA7" s="61"/>
+      <c r="BB7" s="61"/>
+      <c r="BC7" s="61"/>
+      <c r="BD7" s="61"/>
+      <c r="BE7" s="61"/>
+      <c r="BF7" s="61"/>
+      <c r="BG7" s="61"/>
+      <c r="BH7" s="61"/>
+      <c r="BI7" s="61"/>
+      <c r="BJ7" s="61"/>
     </row>
     <row r="8" spans="1:62" ht="9.75" customHeight="1" thickBot="1">
       <c r="U8" s="1"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="53"/>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="54"/>
-      <c r="Z8" s="54"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="53"/>
-      <c r="AC8" s="54"/>
-      <c r="AD8" s="54"/>
-      <c r="AE8" s="54"/>
-      <c r="AF8" s="52"/>
-      <c r="AG8" s="53"/>
-      <c r="AH8" s="53"/>
-      <c r="AI8" s="54"/>
-      <c r="AJ8" s="54"/>
-      <c r="AK8" s="54"/>
-      <c r="AL8" s="68"/>
-      <c r="AM8" s="69"/>
-      <c r="AN8" s="70"/>
-      <c r="AO8" s="70"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="47"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="48"/>
+      <c r="AA8" s="46"/>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="48"/>
+      <c r="AD8" s="48"/>
+      <c r="AE8" s="48"/>
+      <c r="AF8" s="46"/>
+      <c r="AG8" s="47"/>
+      <c r="AH8" s="47"/>
+      <c r="AI8" s="48"/>
+      <c r="AJ8" s="48"/>
+      <c r="AK8" s="48"/>
+      <c r="AL8" s="77"/>
+      <c r="AM8" s="78"/>
+      <c r="AN8" s="79"/>
+      <c r="AO8" s="79"/>
     </row>
     <row r="9" spans="1:62" ht="12.2" customHeight="1" thickBot="1">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="29"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="39"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="30" t="s">
+      <c r="V9" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="W9" s="31" t="s">
+      <c r="W9" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="X9" s="29" t="s">
+      <c r="X9" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="29"/>
-      <c r="AA9" s="30"/>
-      <c r="AB9" s="29"/>
-      <c r="AC9" s="30"/>
-      <c r="AD9" s="29"/>
-      <c r="AE9" s="30"/>
-      <c r="AF9" s="29"/>
-      <c r="AG9" s="30"/>
-      <c r="AH9" s="29"/>
-      <c r="AI9" s="30"/>
-      <c r="AJ9" s="29"/>
-      <c r="AK9" s="30"/>
-      <c r="AL9" s="29"/>
-      <c r="AM9" s="30"/>
-      <c r="AN9" s="29"/>
-      <c r="AO9" s="66"/>
-      <c r="AQ9" s="45" t="s">
+      <c r="Y9" s="40"/>
+      <c r="Z9" s="39"/>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="39"/>
+      <c r="AC9" s="40"/>
+      <c r="AD9" s="39"/>
+      <c r="AE9" s="40"/>
+      <c r="AF9" s="39"/>
+      <c r="AG9" s="40"/>
+      <c r="AH9" s="39"/>
+      <c r="AI9" s="40"/>
+      <c r="AJ9" s="39"/>
+      <c r="AK9" s="40"/>
+      <c r="AL9" s="39"/>
+      <c r="AM9" s="40"/>
+      <c r="AN9" s="39"/>
+      <c r="AO9" s="50"/>
+      <c r="AQ9" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="AR9" s="45"/>
-      <c r="AS9" s="45"/>
-      <c r="AT9" s="45"/>
-      <c r="AU9" s="45"/>
-      <c r="AV9" s="45" t="s">
+      <c r="AR9" s="61"/>
+      <c r="AS9" s="61"/>
+      <c r="AT9" s="61"/>
+      <c r="AU9" s="61"/>
+      <c r="AV9" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="AW9" s="45"/>
-      <c r="AX9" s="45"/>
-      <c r="AY9" s="45"/>
-      <c r="AZ9" s="45"/>
-      <c r="BA9" s="45" t="s">
+      <c r="AW9" s="61"/>
+      <c r="AX9" s="61"/>
+      <c r="AY9" s="61"/>
+      <c r="AZ9" s="61"/>
+      <c r="BA9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="BB9" s="45"/>
-      <c r="BC9" s="45"/>
-      <c r="BD9" s="45"/>
-      <c r="BE9" s="45"/>
-      <c r="BF9" s="45"/>
-      <c r="BG9" s="45" t="s">
+      <c r="BB9" s="61"/>
+      <c r="BC9" s="61"/>
+      <c r="BD9" s="61"/>
+      <c r="BE9" s="61"/>
+      <c r="BF9" s="61"/>
+      <c r="BG9" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="BH9" s="45"/>
-      <c r="BI9" s="45"/>
-      <c r="BJ9" s="45"/>
+      <c r="BH9" s="61"/>
+      <c r="BI9" s="61"/>
+      <c r="BJ9" s="61"/>
     </row>
     <row r="10" spans="1:62" ht="12.2" customHeight="1" thickBot="1">
-      <c r="A10" s="63"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="86" t="s">
+      <c r="A10" s="70"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="87"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="87"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="87"/>
-      <c r="M10" s="87"/>
-      <c r="N10" s="87"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="87"/>
-      <c r="Q10" s="87"/>
-      <c r="R10" s="87"/>
-      <c r="S10" s="87"/>
-      <c r="T10" s="88"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="74"/>
       <c r="U10" s="3"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="67"/>
-      <c r="X10" s="88" t="s">
+      <c r="V10" s="42"/>
+      <c r="W10" s="76"/>
+      <c r="X10" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="Y10" s="89"/>
-      <c r="Z10" s="87"/>
-      <c r="AA10" s="87"/>
-      <c r="AB10" s="87"/>
-      <c r="AC10" s="87"/>
-      <c r="AD10" s="87"/>
-      <c r="AE10" s="87"/>
-      <c r="AF10" s="87"/>
-      <c r="AG10" s="87"/>
-      <c r="AH10" s="87"/>
-      <c r="AI10" s="87"/>
-      <c r="AJ10" s="87"/>
-      <c r="AK10" s="87"/>
-      <c r="AL10" s="87"/>
-      <c r="AM10" s="87"/>
-      <c r="AN10" s="87"/>
-      <c r="AO10" s="87"/>
+      <c r="Y10" s="75"/>
+      <c r="Z10" s="43"/>
+      <c r="AA10" s="43"/>
+      <c r="AB10" s="43"/>
+      <c r="AC10" s="43"/>
+      <c r="AD10" s="43"/>
+      <c r="AE10" s="43"/>
+      <c r="AF10" s="43"/>
+      <c r="AG10" s="43"/>
+      <c r="AH10" s="43"/>
+      <c r="AI10" s="43"/>
+      <c r="AJ10" s="43"/>
+      <c r="AK10" s="43"/>
+      <c r="AL10" s="43"/>
+      <c r="AM10" s="43"/>
+      <c r="AN10" s="43"/>
+      <c r="AO10" s="43"/>
     </row>
     <row r="11" spans="1:62" ht="9.75" customHeight="1" thickTop="1">
-      <c r="AQ11" s="28" t="s">
+      <c r="AQ11" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="AR11" s="28"/>
+      <c r="AR11" s="68"/>
       <c r="AS11" s="5"/>
       <c r="AT11" s="5"/>
       <c r="AU11" s="5"/>
       <c r="AV11" s="5"/>
       <c r="AW11" s="5"/>
       <c r="AX11" s="5"/>
-      <c r="AY11" s="23"/>
-      <c r="AZ11" s="23"/>
-      <c r="BA11" s="23"/>
-      <c r="BB11" s="23"/>
-      <c r="BC11" s="23"/>
-      <c r="BD11" s="24"/>
-      <c r="BE11" s="25"/>
-      <c r="BF11" s="26"/>
-      <c r="BG11" s="25"/>
-      <c r="BH11" s="26"/>
-      <c r="BI11" s="25"/>
-      <c r="BJ11" s="27"/>
+      <c r="AY11" s="34"/>
+      <c r="AZ11" s="34"/>
+      <c r="BA11" s="34"/>
+      <c r="BB11" s="34"/>
+      <c r="BC11" s="34"/>
+      <c r="BD11" s="35"/>
+      <c r="BE11" s="36"/>
+      <c r="BF11" s="37"/>
+      <c r="BG11" s="36"/>
+      <c r="BH11" s="37"/>
+      <c r="BI11" s="36"/>
+      <c r="BJ11" s="38"/>
     </row>
     <row r="12" spans="1:62" ht="9.75" customHeight="1">
-      <c r="AQ12" s="46"/>
-      <c r="AR12" s="46"/>
+      <c r="AQ12" s="62"/>
+      <c r="AR12" s="62"/>
       <c r="AS12" s="6"/>
       <c r="AT12" s="6"/>
       <c r="AU12" s="6"/>
       <c r="AV12" s="6"/>
       <c r="AW12" s="6"/>
       <c r="AX12" s="6"/>
-      <c r="AY12" s="47"/>
-      <c r="AZ12" s="47"/>
-      <c r="BA12" s="47"/>
-      <c r="BB12" s="47"/>
-      <c r="BC12" s="47"/>
-      <c r="BD12" s="48"/>
-      <c r="BE12" s="49"/>
-      <c r="BF12" s="50"/>
-      <c r="BG12" s="49"/>
-      <c r="BH12" s="50"/>
-      <c r="BI12" s="49"/>
-      <c r="BJ12" s="51"/>
+      <c r="AY12" s="63"/>
+      <c r="AZ12" s="63"/>
+      <c r="BA12" s="63"/>
+      <c r="BB12" s="63"/>
+      <c r="BC12" s="63"/>
+      <c r="BD12" s="64"/>
+      <c r="BE12" s="65"/>
+      <c r="BF12" s="66"/>
+      <c r="BG12" s="65"/>
+      <c r="BH12" s="66"/>
+      <c r="BI12" s="65"/>
+      <c r="BJ12" s="67"/>
     </row>
     <row r="14" spans="1:62" ht="9.75" customHeight="1">
-      <c r="AQ14" s="33"/>
-      <c r="AR14" s="34"/>
+      <c r="AQ14" s="44"/>
+      <c r="AR14" s="45"/>
     </row>
     <row r="15" spans="1:62" ht="11.45" customHeight="1">
-      <c r="AQ15" s="35"/>
-      <c r="AR15" s="36"/>
+      <c r="AQ15" s="51"/>
+      <c r="AR15" s="52"/>
     </row>
     <row r="16" spans="1:62" ht="11.45" customHeight="1">
-      <c r="AQ16" s="37"/>
-      <c r="AR16" s="38"/>
+      <c r="AQ16" s="53"/>
+      <c r="AR16" s="54"/>
     </row>
     <row r="17" spans="43:44" ht="11.45" customHeight="1">
-      <c r="AQ17" s="39"/>
-      <c r="AR17" s="40"/>
+      <c r="AQ17" s="55"/>
+      <c r="AR17" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="175">
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BG1:BH1"/>
     <mergeCell ref="BI2:BJ2"/>
     <mergeCell ref="BG2:BH2"/>
     <mergeCell ref="BE2:BF2"/>
@@ -1951,8 +1950,14 @@
     <mergeCell ref="BA2:BB2"/>
     <mergeCell ref="AY2:AZ2"/>
     <mergeCell ref="AW2:AX2"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AR1:AR2"/>
+    <mergeCell ref="AQ1:AQ2"/>
+    <mergeCell ref="AJ4:AK4"/>
+    <mergeCell ref="AL4:AM4"/>
+    <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AD5:AE7"/>
     <mergeCell ref="BE1:BF1"/>
     <mergeCell ref="BC1:BD1"/>
     <mergeCell ref="BA1:BB1"/>
@@ -1960,8 +1965,13 @@
     <mergeCell ref="AW1:AX1"/>
     <mergeCell ref="AU1:AV1"/>
     <mergeCell ref="AS1:AT1"/>
-    <mergeCell ref="BI1:BJ1"/>
-    <mergeCell ref="BG1:BH1"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="AD10:AE10"/>
     <mergeCell ref="AA8:AE8"/>
     <mergeCell ref="AF8:AK8"/>
     <mergeCell ref="AL8:AO8"/>
@@ -1970,23 +1980,6 @@
     <mergeCell ref="AJ5:AK7"/>
     <mergeCell ref="AL5:AM7"/>
     <mergeCell ref="AN5:AO7"/>
-    <mergeCell ref="AR1:AR2"/>
-    <mergeCell ref="AQ1:AQ2"/>
-    <mergeCell ref="AJ4:AK4"/>
-    <mergeCell ref="AL4:AM4"/>
-    <mergeCell ref="AN4:AO4"/>
-    <mergeCell ref="AH4:AI4"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="X10:Y10"/>
-    <mergeCell ref="Z10:AA10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="AD9:AE9"/>
-    <mergeCell ref="AB10:AC10"/>
-    <mergeCell ref="AD10:AE10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:D9"/>
@@ -2013,6 +2006,9 @@
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
     <mergeCell ref="AQ15:AR17"/>
     <mergeCell ref="AQ4:AQ5"/>
     <mergeCell ref="AR4:AR5"/>
@@ -2036,8 +2032,6 @@
     <mergeCell ref="BE5:BF5"/>
     <mergeCell ref="AW5:AX5"/>
     <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AQ11:AR11"/>
-    <mergeCell ref="AY4:AZ4"/>
     <mergeCell ref="Z9:AA9"/>
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="S9:T9"/>
@@ -2048,10 +2042,6 @@
     <mergeCell ref="V8:Z8"/>
     <mergeCell ref="U7:V7"/>
     <mergeCell ref="W7:X7"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="U5:V5"/>
     <mergeCell ref="AL10:AM10"/>
     <mergeCell ref="AN10:AO10"/>
     <mergeCell ref="AH9:AI9"/>
@@ -2060,6 +2050,12 @@
     <mergeCell ref="AN9:AO9"/>
     <mergeCell ref="AF9:AG9"/>
     <mergeCell ref="AF10:AG10"/>
+    <mergeCell ref="AQ11:AR11"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="Z10:AA10"/>
+    <mergeCell ref="W9:W10"/>
     <mergeCell ref="BI5:BJ5"/>
     <mergeCell ref="AY11:AZ11"/>
     <mergeCell ref="BA11:BB11"/>
@@ -2069,13 +2065,19 @@
     <mergeCell ref="BG11:BH11"/>
     <mergeCell ref="BI11:BJ11"/>
     <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="BE4:BF4"/>
+    <mergeCell ref="BG4:BH4"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="BG5:BH5"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
@@ -2090,22 +2092,6 @@
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="S7:T7"/>
     <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="BE4:BF4"/>
-    <mergeCell ref="BG4:BH4"/>
-    <mergeCell ref="AD5:AE7"/>
-    <mergeCell ref="AS5:AT5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="BG5:BH5"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="K1:T1"/>
     <mergeCell ref="A2:J2"/>
@@ -2119,6 +2105,17 @@
     <mergeCell ref="A4:B7"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:J3"/>
+    <mergeCell ref="AS5:AT5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="U5:V5"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>